<commit_message>
cambio de nanos a micros
</commit_message>
<xml_diff>
--- a/JProfiler/Tablas de Tiempos.xlsx
+++ b/JProfiler/Tablas de Tiempos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Documents\GitHub\HdT3\JProfiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3EAC2E-63F1-4F5D-8566-D3771BF07F5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DC0224-E467-42EE-BB60-73FC01FC01F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D3DF4C85-E1E4-4B46-A9CD-5D936FB701F1}"/>
   </bookViews>
@@ -185,7 +185,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-GT"/>
-              <a:t>Items Desordenados vs Nanosegundos</a:t>
+              <a:t>Items Desordenados vs Microsegundos</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -797,7 +797,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-GT"/>
-                  <a:t>Nanosegundos</a:t>
+                  <a:t>Microsegundos</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -987,7 +987,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="es-GT" baseline="0"/>
-              <a:t> vs Nanosegundos</a:t>
+              <a:t> vs Microsegundos</a:t>
             </a:r>
             <a:endParaRPr lang="es-GT"/>
           </a:p>
@@ -1603,7 +1603,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-GT"/>
-                  <a:t>Nanosegundos</a:t>
+                  <a:t>Microsegundos</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3242,8 +3242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2DED0E3-8450-44E9-9671-01B3752DA6AE}">
   <dimension ref="C3:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="Q45" sqref="Q45"/>
+    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3380,7 +3380,7 @@
         <v>52125</v>
       </c>
       <c r="G6" s="3">
-        <v>358000000</v>
+        <v>358000</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>2</v>
@@ -3444,7 +3444,7 @@
         <v>83479</v>
       </c>
       <c r="G8" s="3">
-        <v>704000000</v>
+        <v>704000</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>4</v>
@@ -3459,7 +3459,7 @@
         <v>70710</v>
       </c>
       <c r="M8" s="2">
-        <v>558000000</v>
+        <v>558000</v>
       </c>
     </row>
     <row r="11" spans="3:15" x14ac:dyDescent="0.35">

</xml_diff>